<commit_message>
add code for TPAF salary table
</commit_message>
<xml_diff>
--- a/Data/TPAF ES2012 Assumptions.xlsx
+++ b/Data/TPAF ES2012 Assumptions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" state="visible" r:id="rId2"/>
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="96">
   <si>
     <t>Table of Contents</t>
   </si>
@@ -3313,7 +3313,7 @@
   </sheetPr>
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="U17" activeCellId="0" sqref="U17"/>
     </sheetView>
   </sheetViews>
@@ -6362,7 +6362,7 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -8296,8 +8296,8 @@
   </sheetPr>
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D100" activeCellId="0" sqref="D100"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A81" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G59" activeCellId="0" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9680,20 +9680,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="n">
-        <v>110</v>
-      </c>
-      <c r="B100" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C100" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D100" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:D2"/>

</xml_diff>

<commit_message>
add code for importing termination rates(general and class A/B)
</commit_message>
<xml_diff>
--- a/Data/TPAF ES2012 Assumptions.xlsx
+++ b/Data/TPAF ES2012 Assumptions.xlsx
@@ -274,7 +274,7 @@
     <t>Term Rate</t>
   </si>
   <si>
-    <t>Term</t>
+    <t>qxt.rf.lt10</t>
   </si>
   <si>
     <t>10-14 yos</t>
@@ -298,31 +298,31 @@
     <t>age</t>
   </si>
   <si>
-    <t>vested10_14</t>
+    <t>qxt.vest.10_14</t>
   </si>
   <si>
-    <t>refund10_14</t>
+    <t>qxt.rf.10_14</t>
   </si>
   <si>
-    <t>vested15_19</t>
+    <t>qxt.vest.15_19</t>
   </si>
   <si>
-    <t>refund15_19</t>
+    <t>qxt.rf.15_19</t>
   </si>
   <si>
-    <t>vested20_24</t>
+    <t>qxt.vest.20_24</t>
   </si>
   <si>
-    <t>refund20_24</t>
+    <t>qxt.rf.20_24</t>
   </si>
   <si>
     <t>Term Rates</t>
   </si>
   <si>
-    <t>age_lt40</t>
+    <t>qxt.rf.lt10.lt40</t>
   </si>
   <si>
-    <t>age_egt40</t>
+    <t>qxt.rf.lt10.egt40</t>
   </si>
   <si>
     <t>Ordinary Disability</t>
@@ -903,8 +903,8 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4627,7 +4627,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4765,17 +4765,17 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.54081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.219387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4132653061224"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.530612244898"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6683673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.530612244898"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.6683673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.54081632653061"/>
   </cols>
@@ -4822,7 +4822,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>39</v>
       </c>
@@ -5677,12 +5677,15 @@
   <dimension ref="A1:AMI14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.54081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.54081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.54081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6216,7 +6219,7 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>26</v>
       </c>
@@ -6363,7 +6366,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6420,7 +6423,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>39</v>
       </c>
@@ -6719,7 +6722,7 @@
         <v>0.0027</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>37</v>
       </c>
@@ -8296,7 +8299,7 @@
   </sheetPr>
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A81" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G59" activeCellId="0" sqref="G59"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add code for importing mortality and disability rates
</commit_message>
<xml_diff>
--- a/Data/TPAF ES2012 Assumptions.xlsx
+++ b/Data/TPAF ES2012 Assumptions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" state="visible" r:id="rId2"/>
@@ -337,16 +337,16 @@
     <t>Female</t>
   </si>
   <si>
-    <t>disb_o_m</t>
+    <t>qxd_o_m</t>
   </si>
   <si>
-    <t>disb_o_f</t>
+    <t>qxd_o_f</t>
   </si>
   <si>
-    <t>disb_a_m</t>
+    <t>qxd_a_m</t>
   </si>
   <si>
-    <t>disb_a_f</t>
+    <t>qxd_a_f</t>
   </si>
   <si>
     <t>Active</t>
@@ -364,13 +364,13 @@
     <t>Disabled</t>
   </si>
   <si>
-    <t>qm_act_o</t>
+    <t>qxm_act_o</t>
   </si>
   <si>
-    <t>qm_post_h</t>
+    <t>qxm_post_h</t>
   </si>
   <si>
-    <t>qm_post_d</t>
+    <t>qxm_post_d</t>
   </si>
   <si>
     <t>NA</t>
@@ -903,8 +903,8 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4764,7 +4764,7 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -6365,7 +6365,7 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -7277,8 +7277,8 @@
   </sheetPr>
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8300,7 +8300,7 @@
   <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G59" activeCellId="0" sqref="G59"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9709,15 +9709,15 @@
   </sheetPr>
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.54081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.21428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5102040816327"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.54081632653061"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
add code for calculating service retirement AL for class AB, not completed yet.
</commit_message>
<xml_diff>
--- a/Data/TPAF ES2012 Assumptions.xlsx
+++ b/Data/TPAF ES2012 Assumptions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" state="visible" r:id="rId2"/>
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="87">
   <si>
     <t>Table of Contents</t>
   </si>
@@ -408,64 +408,37 @@
 Eligibility</t>
   </si>
   <si>
-    <t>qxr.m_lt25yos_AB</t>
+    <t>qxr_lt25yos_AB</t>
   </si>
   <si>
-    <t>qxr.m_gt25yos_f_AB</t>
+    <t>qxr_gt25yos_f_AB</t>
   </si>
   <si>
-    <t>qxr.m_gt25yos_AB</t>
+    <t>qxr_gt25yos_AB</t>
   </si>
   <si>
-    <t>qxr.m_lt25yos_D</t>
+    <t>qxr_lt25yos_D</t>
   </si>
   <si>
-    <t>qxr.m_gt25yos_f_D</t>
+    <t>qxr_gt25yos_f_D</t>
   </si>
   <si>
-    <t>qxr.m_gt25yos_D</t>
+    <t>qxr_gt25yos_D</t>
   </si>
   <si>
-    <t>qxr.m_lt25yos_EF</t>
+    <t>qxr_lt25yos_EF</t>
   </si>
   <si>
-    <t>qxr.m_gt25yos_f_EF</t>
+    <t>qxr_gt25yos_f_EF</t>
   </si>
   <si>
-    <t>qxr.m_gt25yos_EF</t>
+    <t>qxr_gt25yos_EF</t>
   </si>
   <si>
     <t>Less than 20 yos</t>
   </si>
   <si>
     <t>More than 20 yos</t>
-  </si>
-  <si>
-    <t>qxr.f_lt25yos_AB</t>
-  </si>
-  <si>
-    <t>qxr.f_gt25yos_f_AB</t>
-  </si>
-  <si>
-    <t>qxr.f_gt25yos_AB</t>
-  </si>
-  <si>
-    <t>qxr.f_lt25yos_D</t>
-  </si>
-  <si>
-    <t>qxr.f_gt25yos_f_D</t>
-  </si>
-  <si>
-    <t>qxr.f_gt25yos_D</t>
-  </si>
-  <si>
-    <t>qxr.f_lt25yos_EF</t>
-  </si>
-  <si>
-    <t>qxr.f_gt25yos_f_EF</t>
-  </si>
-  <si>
-    <t>qxr.f_gt25yos_EF</t>
   </si>
 </sst>
 </file>
@@ -903,8 +876,8 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2104,13 +2077,14 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="15" width="8.89285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.54081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.54081632653061"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="12" width="14.3367346938776"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="12" width="15.3367346938776"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="12" width="8.10714285714286"/>
@@ -2224,40 +2198,40 @@
         <v>39</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4764,7 +4738,7 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -7277,8 +7251,8 @@
   </sheetPr>
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
add code for a preliminary calculation of service retirement AL for class A/B
</commit_message>
<xml_diff>
--- a/Data/TPAF ES2012 Assumptions.xlsx
+++ b/Data/TPAF ES2012 Assumptions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" state="visible" r:id="rId2"/>
@@ -876,7 +876,7 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2074,10 +2074,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q14" activeCellId="0" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2439,7 +2439,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="n">
         <v>52</v>
       </c>
@@ -3259,6 +3259,7 @@
         <v>0.3</v>
       </c>
     </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B4:D4"/>
@@ -3287,7 +3288,7 @@
   </sheetPr>
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="U17" activeCellId="0" sqref="U17"/>
     </sheetView>
   </sheetViews>
@@ -8273,7 +8274,7 @@
   </sheetPr>
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>